<commit_message>
commit reglement de dette
</commit_message>
<xml_diff>
--- a/Gesstion ESN 2020/Billan Financier  Journalier.xlsx
+++ b/Gesstion ESN 2020/Billan Financier  Journalier.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ESN FORMATIC\Documents\NOTE INFORMATION ESN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\FORMATIC\FormaTIC Gestion 2021\Adminitratif\gestion cloud integré\esn_formatic\Gesstion ESN 2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17085" windowHeight="7755" tabRatio="598"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17085" windowHeight="7755" tabRatio="598" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Bilan" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="104">
   <si>
     <t>Bilan Financier Journalier</t>
   </si>
@@ -294,19 +294,7 @@
     <t>Mady yameogo</t>
   </si>
   <si>
-    <t>jean noel</t>
-  </si>
-  <si>
-    <t>yanick</t>
-  </si>
-  <si>
     <t>gerard</t>
-  </si>
-  <si>
-    <t>fredo</t>
-  </si>
-  <si>
-    <t>jeremie</t>
   </si>
   <si>
     <t>paul zale</t>
@@ -359,8 +347,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -706,7 +694,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -743,36 +731,36 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="8" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -787,15 +775,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="10" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="10" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="10" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="10" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="10" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="10" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="10" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -817,15 +814,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Milliers" xfId="1" builtinId="3"/>
@@ -1112,9 +1100,9 @@
   </sheetPr>
   <dimension ref="A1:AIV494"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F27" sqref="F27"/>
+      <selection pane="topRight" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,23 +1129,23 @@
       <c r="A2" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="82">
+      <c r="B2" s="75">
         <v>250000</v>
       </c>
-      <c r="C2" s="83">
+      <c r="C2" s="76">
         <v>256803</v>
       </c>
-      <c r="D2" s="83">
+      <c r="D2" s="76">
         <v>187803</v>
       </c>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
-      <c r="L2" s="83"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="76"/>
       <c r="M2" s="66"/>
       <c r="N2" s="66"/>
       <c r="O2" s="66"/>
@@ -2083,23 +2071,23 @@
       <c r="A3" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="82">
+      <c r="B3" s="75">
         <v>50000</v>
       </c>
-      <c r="C3" s="83">
+      <c r="C3" s="76">
         <v>138559.73000000001</v>
       </c>
-      <c r="D3" s="83">
+      <c r="D3" s="76">
         <v>101209.73</v>
       </c>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="83"/>
-      <c r="L3" s="83"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
       <c r="M3" s="66"/>
       <c r="N3" s="66"/>
       <c r="O3" s="66"/>
@@ -3025,23 +3013,23 @@
       <c r="A4" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="82">
+      <c r="B4" s="75">
         <v>300000</v>
       </c>
-      <c r="C4" s="83">
+      <c r="C4" s="76">
         <v>287000</v>
       </c>
-      <c r="D4" s="83">
+      <c r="D4" s="76">
         <v>353400</v>
       </c>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="76"/>
       <c r="M4" s="66"/>
       <c r="N4" s="66"/>
       <c r="O4" s="66"/>
@@ -3967,23 +3955,23 @@
       <c r="A5" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="82">
+      <c r="B5" s="75">
         <v>0</v>
       </c>
-      <c r="C5" s="83">
+      <c r="C5" s="76">
         <v>100000</v>
       </c>
-      <c r="D5" s="83">
+      <c r="D5" s="76">
         <v>100000</v>
       </c>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="83"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="76"/>
+      <c r="L5" s="76"/>
       <c r="M5" s="66"/>
       <c r="N5" s="66"/>
       <c r="O5" s="66"/>
@@ -4909,47 +4897,47 @@
       <c r="A6" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="82">
+      <c r="B6" s="75">
         <f>SUM(B2:B4)-B5</f>
         <v>600000</v>
       </c>
-      <c r="C6" s="84">
+      <c r="C6" s="77">
         <f t="shared" ref="C6:P6" si="0">SUM(C2:C4)-C5</f>
         <v>582362.73</v>
       </c>
-      <c r="D6" s="84">
+      <c r="D6" s="77">
         <f t="shared" si="0"/>
         <v>542412.73</v>
       </c>
-      <c r="E6" s="84">
+      <c r="E6" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F6" s="84">
+      <c r="F6" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G6" s="84">
+      <c r="G6" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="84">
+      <c r="H6" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I6" s="84">
+      <c r="I6" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J6" s="84">
+      <c r="J6" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K6" s="84">
+      <c r="K6" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L6" s="84">
+      <c r="L6" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5888,65 +5876,64 @@
     </row>
     <row r="7" spans="1:932" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="61" t="s">
-        <v>96</v>
-      </c>
-      <c r="B7" s="82">
+        <v>92</v>
+      </c>
+      <c r="B7" s="75">
         <v>0</v>
       </c>
-      <c r="C7" s="84">
+      <c r="C7" s="77">
         <v>86000</v>
       </c>
-      <c r="D7" s="84">
+      <c r="D7" s="77">
+        <v>130000</v>
+      </c>
+      <c r="E7" s="77">
         <f>'dette transfert'!$D$4</f>
-        <v>130000</v>
-      </c>
-      <c r="E7" s="84">
+        <v>120000</v>
+      </c>
+      <c r="F7" s="77">
         <f>'dette transfert'!$D$4</f>
-        <v>130000</v>
-      </c>
-      <c r="F7" s="84">
+        <v>120000</v>
+      </c>
+      <c r="G7" s="77">
         <f>'dette transfert'!$D$4</f>
-        <v>130000</v>
-      </c>
-      <c r="G7" s="84">
+        <v>120000</v>
+      </c>
+      <c r="H7" s="77">
         <f>'dette transfert'!$D$4</f>
-        <v>130000</v>
-      </c>
-      <c r="H7" s="84">
+        <v>120000</v>
+      </c>
+      <c r="I7" s="77">
         <f>'dette transfert'!$D$4</f>
-        <v>130000</v>
-      </c>
-      <c r="I7" s="84">
+        <v>120000</v>
+      </c>
+      <c r="J7" s="77">
         <f>'dette transfert'!$D$4</f>
-        <v>130000</v>
-      </c>
-      <c r="J7" s="84">
+        <v>120000</v>
+      </c>
+      <c r="K7" s="77">
         <f>'dette transfert'!$D$4</f>
-        <v>130000</v>
-      </c>
-      <c r="K7" s="84">
+        <v>120000</v>
+      </c>
+      <c r="L7" s="77">
         <f>'dette transfert'!$D$4</f>
-        <v>130000</v>
-      </c>
-      <c r="L7" s="84">
-        <f>'dette transfert'!$D$4</f>
-        <v>130000</v>
+        <v>120000</v>
       </c>
       <c r="M7" s="67">
         <f>'dette transfert'!$D$4</f>
-        <v>130000</v>
+        <v>120000</v>
       </c>
       <c r="N7" s="67">
         <f>'dette transfert'!$D$4</f>
-        <v>130000</v>
+        <v>120000</v>
       </c>
       <c r="O7" s="67">
         <f>'dette transfert'!$D$4</f>
-        <v>130000</v>
+        <v>120000</v>
       </c>
       <c r="P7" s="67">
         <f>'dette transfert'!$D$4</f>
-        <v>130000</v>
+        <v>120000</v>
       </c>
       <c r="Q7" s="67"/>
       <c r="R7" s="67"/>
@@ -6867,67 +6854,67 @@
     </row>
     <row r="8" spans="1:932" s="57" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="62" t="s">
-        <v>97</v>
-      </c>
-      <c r="B8" s="85">
+        <v>93</v>
+      </c>
+      <c r="B8" s="78">
         <f>B6+B7</f>
         <v>600000</v>
       </c>
-      <c r="C8" s="86">
+      <c r="C8" s="79">
         <f>C6+C7</f>
         <v>668362.73</v>
       </c>
-      <c r="D8" s="86">
+      <c r="D8" s="79">
         <f t="shared" ref="D8:P8" si="1">D6+D7</f>
         <v>672412.73</v>
       </c>
-      <c r="E8" s="86">
+      <c r="E8" s="79">
         <f t="shared" si="1"/>
-        <v>130000</v>
-      </c>
-      <c r="F8" s="86">
+        <v>120000</v>
+      </c>
+      <c r="F8" s="79">
         <f t="shared" si="1"/>
-        <v>130000</v>
-      </c>
-      <c r="G8" s="86">
+        <v>120000</v>
+      </c>
+      <c r="G8" s="79">
         <f t="shared" si="1"/>
-        <v>130000</v>
-      </c>
-      <c r="H8" s="86">
+        <v>120000</v>
+      </c>
+      <c r="H8" s="79">
         <f t="shared" si="1"/>
-        <v>130000</v>
-      </c>
-      <c r="I8" s="86">
+        <v>120000</v>
+      </c>
+      <c r="I8" s="79">
         <f t="shared" si="1"/>
-        <v>130000</v>
-      </c>
-      <c r="J8" s="86">
+        <v>120000</v>
+      </c>
+      <c r="J8" s="79">
         <f t="shared" si="1"/>
-        <v>130000</v>
-      </c>
-      <c r="K8" s="86">
+        <v>120000</v>
+      </c>
+      <c r="K8" s="79">
         <f t="shared" si="1"/>
-        <v>130000</v>
-      </c>
-      <c r="L8" s="86">
+        <v>120000</v>
+      </c>
+      <c r="L8" s="79">
         <f t="shared" si="1"/>
-        <v>130000</v>
+        <v>120000</v>
       </c>
       <c r="M8" s="68">
         <f t="shared" si="1"/>
-        <v>130000</v>
+        <v>120000</v>
       </c>
       <c r="N8" s="68">
         <f t="shared" si="1"/>
-        <v>130000</v>
+        <v>120000</v>
       </c>
       <c r="O8" s="68">
         <f t="shared" si="1"/>
-        <v>130000</v>
+        <v>120000</v>
       </c>
       <c r="P8" s="68">
         <f t="shared" si="1"/>
-        <v>130000</v>
+        <v>120000</v>
       </c>
       <c r="Q8" s="68"/>
       <c r="R8" s="68"/>
@@ -7847,17 +7834,17 @@
       <c r="AIV8" s="68"/>
     </row>
     <row r="9" spans="1:932" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="87"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="88"/>
-      <c r="E9" s="88"/>
-      <c r="F9" s="88"/>
-      <c r="G9" s="88"/>
-      <c r="H9" s="88"/>
-      <c r="I9" s="88"/>
-      <c r="J9" s="88"/>
-      <c r="K9" s="88"/>
-      <c r="L9" s="88"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="81"/>
+      <c r="G9" s="81"/>
+      <c r="H9" s="81"/>
+      <c r="I9" s="81"/>
+      <c r="J9" s="81"/>
+      <c r="K9" s="81"/>
+      <c r="L9" s="81"/>
       <c r="M9" s="69"/>
       <c r="N9" s="69"/>
       <c r="O9" s="69"/>
@@ -8780,17 +8767,17 @@
       <c r="AIV9" s="69"/>
     </row>
     <row r="10" spans="1:932" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="87"/>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="88"/>
-      <c r="H10" s="88"/>
-      <c r="I10" s="88"/>
-      <c r="J10" s="88"/>
-      <c r="K10" s="88"/>
-      <c r="L10" s="88"/>
+      <c r="B10" s="80"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="81"/>
+      <c r="H10" s="81"/>
+      <c r="I10" s="81"/>
+      <c r="J10" s="81"/>
+      <c r="K10" s="81"/>
+      <c r="L10" s="81"/>
       <c r="M10" s="69"/>
       <c r="N10" s="69"/>
       <c r="O10" s="69"/>
@@ -9713,17 +9700,17 @@
       <c r="AIV10" s="69"/>
     </row>
     <row r="11" spans="1:932" s="55" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="87"/>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="88"/>
-      <c r="J11" s="88"/>
-      <c r="K11" s="88"/>
-      <c r="L11" s="88"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="81"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="81"/>
+      <c r="L11" s="81"/>
       <c r="M11" s="69"/>
       <c r="N11" s="69"/>
       <c r="O11" s="69"/>
@@ -10647,23 +10634,23 @@
     </row>
     <row r="12" spans="1:932" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="59" t="s">
-        <v>98</v>
-      </c>
-      <c r="B12" s="89">
+        <v>94</v>
+      </c>
+      <c r="B12" s="82">
         <v>5000</v>
       </c>
-      <c r="C12" s="90"/>
-      <c r="D12" s="90">
+      <c r="C12" s="83"/>
+      <c r="D12" s="83">
         <v>3775</v>
       </c>
-      <c r="E12" s="90"/>
-      <c r="F12" s="90"/>
-      <c r="G12" s="90"/>
-      <c r="H12" s="90"/>
-      <c r="I12" s="90"/>
-      <c r="J12" s="90"/>
-      <c r="K12" s="90"/>
-      <c r="L12" s="90"/>
+      <c r="E12" s="83"/>
+      <c r="F12" s="83"/>
+      <c r="G12" s="83"/>
+      <c r="H12" s="83"/>
+      <c r="I12" s="83"/>
+      <c r="J12" s="83"/>
+      <c r="K12" s="83"/>
+      <c r="L12" s="83"/>
       <c r="M12" s="70"/>
       <c r="N12" s="70"/>
       <c r="O12" s="70"/>
@@ -11587,23 +11574,23 @@
     </row>
     <row r="13" spans="1:932" x14ac:dyDescent="0.25">
       <c r="A13" s="60" t="s">
-        <v>99</v>
-      </c>
-      <c r="B13" s="82">
+        <v>95</v>
+      </c>
+      <c r="B13" s="75">
         <v>25000</v>
       </c>
-      <c r="C13" s="83"/>
-      <c r="D13" s="83">
+      <c r="C13" s="76"/>
+      <c r="D13" s="76">
         <v>16887.5</v>
       </c>
-      <c r="E13" s="83"/>
-      <c r="F13" s="83"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="83"/>
-      <c r="I13" s="83"/>
-      <c r="J13" s="83"/>
-      <c r="K13" s="83"/>
-      <c r="L13" s="83"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="76"/>
+      <c r="I13" s="76"/>
+      <c r="J13" s="76"/>
+      <c r="K13" s="76"/>
+      <c r="L13" s="76"/>
       <c r="M13" s="66"/>
       <c r="N13" s="66"/>
       <c r="O13" s="66"/>
@@ -12527,23 +12514,23 @@
     </row>
     <row r="14" spans="1:932" x14ac:dyDescent="0.25">
       <c r="A14" s="60" t="s">
-        <v>100</v>
-      </c>
-      <c r="B14" s="82">
+        <v>96</v>
+      </c>
+      <c r="B14" s="75">
         <v>5000</v>
       </c>
-      <c r="C14" s="83"/>
-      <c r="D14" s="83">
+      <c r="C14" s="76"/>
+      <c r="D14" s="76">
         <v>3600</v>
       </c>
-      <c r="E14" s="83"/>
-      <c r="F14" s="83"/>
-      <c r="G14" s="83"/>
-      <c r="H14" s="83"/>
-      <c r="I14" s="83"/>
-      <c r="J14" s="83"/>
-      <c r="K14" s="83"/>
-      <c r="L14" s="83"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="76"/>
+      <c r="I14" s="76"/>
+      <c r="J14" s="76"/>
+      <c r="K14" s="76"/>
+      <c r="L14" s="76"/>
       <c r="M14" s="66"/>
       <c r="N14" s="66"/>
       <c r="O14" s="66"/>
@@ -13467,25 +13454,25 @@
     </row>
     <row r="15" spans="1:932" x14ac:dyDescent="0.25">
       <c r="A15" s="60" t="s">
-        <v>101</v>
-      </c>
-      <c r="B15" s="82">
+        <v>97</v>
+      </c>
+      <c r="B15" s="75">
         <v>25000</v>
       </c>
-      <c r="C15" s="83">
+      <c r="C15" s="76">
         <v>3897</v>
       </c>
-      <c r="D15" s="83">
+      <c r="D15" s="76">
         <v>3897</v>
       </c>
-      <c r="E15" s="83"/>
-      <c r="F15" s="83"/>
-      <c r="G15" s="83"/>
-      <c r="H15" s="83"/>
-      <c r="I15" s="83"/>
-      <c r="J15" s="83"/>
-      <c r="K15" s="83"/>
-      <c r="L15" s="83"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="76"/>
+      <c r="J15" s="76"/>
+      <c r="K15" s="76"/>
+      <c r="L15" s="76"/>
       <c r="M15" s="66"/>
       <c r="N15" s="66"/>
       <c r="O15" s="66"/>
@@ -14409,23 +14396,23 @@
     </row>
     <row r="16" spans="1:932" x14ac:dyDescent="0.25">
       <c r="A16" s="60" t="s">
-        <v>103</v>
-      </c>
-      <c r="B16" s="82">
+        <v>99</v>
+      </c>
+      <c r="B16" s="75">
         <v>10000</v>
       </c>
-      <c r="C16" s="83"/>
-      <c r="D16" s="83">
+      <c r="C16" s="76"/>
+      <c r="D16" s="76">
         <v>5892.54</v>
       </c>
-      <c r="E16" s="83"/>
-      <c r="F16" s="83"/>
-      <c r="G16" s="83"/>
-      <c r="H16" s="83"/>
-      <c r="I16" s="83"/>
-      <c r="J16" s="83"/>
-      <c r="K16" s="83"/>
-      <c r="L16" s="83"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="76"/>
+      <c r="I16" s="76"/>
+      <c r="J16" s="76"/>
+      <c r="K16" s="76"/>
+      <c r="L16" s="76"/>
       <c r="M16" s="66"/>
       <c r="N16" s="66"/>
       <c r="O16" s="66"/>
@@ -15349,23 +15336,23 @@
     </row>
     <row r="17" spans="1:932" x14ac:dyDescent="0.25">
       <c r="A17" s="60" t="s">
-        <v>102</v>
-      </c>
-      <c r="B17" s="82">
+        <v>98</v>
+      </c>
+      <c r="B17" s="75">
         <v>0</v>
       </c>
-      <c r="C17" s="83"/>
-      <c r="D17" s="83">
+      <c r="C17" s="76"/>
+      <c r="D17" s="76">
         <v>39875</v>
       </c>
-      <c r="E17" s="83"/>
-      <c r="F17" s="83"/>
-      <c r="G17" s="83"/>
-      <c r="H17" s="83"/>
-      <c r="I17" s="83"/>
-      <c r="J17" s="83"/>
-      <c r="K17" s="83"/>
-      <c r="L17" s="83"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
+      <c r="H17" s="76"/>
+      <c r="I17" s="76"/>
+      <c r="J17" s="76"/>
+      <c r="K17" s="76"/>
+      <c r="L17" s="76"/>
       <c r="M17" s="66"/>
       <c r="N17" s="66"/>
       <c r="O17" s="66"/>
@@ -16291,47 +16278,47 @@
       <c r="A18" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="82">
+      <c r="B18" s="75">
         <f>SUM(B12:B17)</f>
         <v>70000</v>
       </c>
-      <c r="C18" s="84">
+      <c r="C18" s="77">
         <f t="shared" ref="C18:P18" si="2">SUM(C12:C17)</f>
         <v>3897</v>
       </c>
-      <c r="D18" s="84">
+      <c r="D18" s="77">
         <f t="shared" si="2"/>
         <v>73927.040000000008</v>
       </c>
-      <c r="E18" s="84">
+      <c r="E18" s="77">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F18" s="84">
+      <c r="F18" s="77">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G18" s="84">
+      <c r="G18" s="77">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H18" s="84">
+      <c r="H18" s="77">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I18" s="84">
+      <c r="I18" s="77">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J18" s="84">
+      <c r="J18" s="77">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K18" s="84">
+      <c r="K18" s="77">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L18" s="84">
+      <c r="L18" s="77">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -17270,65 +17257,64 @@
     </row>
     <row r="19" spans="1:932" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="61" t="s">
-        <v>96</v>
-      </c>
-      <c r="B19" s="82">
+        <v>92</v>
+      </c>
+      <c r="B19" s="75">
         <v>0</v>
       </c>
-      <c r="C19" s="84">
+      <c r="C19" s="77">
         <v>40350</v>
       </c>
-      <c r="D19" s="84">
+      <c r="D19" s="77">
+        <v>37050</v>
+      </c>
+      <c r="E19" s="77">
         <f>'dette unite'!$D$4</f>
-        <v>37050</v>
-      </c>
-      <c r="E19" s="84">
+        <v>34050</v>
+      </c>
+      <c r="F19" s="77">
         <f>'dette unite'!$D$4</f>
-        <v>37050</v>
-      </c>
-      <c r="F19" s="84">
+        <v>34050</v>
+      </c>
+      <c r="G19" s="77">
         <f>'dette unite'!$D$4</f>
-        <v>37050</v>
-      </c>
-      <c r="G19" s="84">
+        <v>34050</v>
+      </c>
+      <c r="H19" s="77">
         <f>'dette unite'!$D$4</f>
-        <v>37050</v>
-      </c>
-      <c r="H19" s="84">
+        <v>34050</v>
+      </c>
+      <c r="I19" s="77">
         <f>'dette unite'!$D$4</f>
-        <v>37050</v>
-      </c>
-      <c r="I19" s="84">
+        <v>34050</v>
+      </c>
+      <c r="J19" s="77">
         <f>'dette unite'!$D$4</f>
-        <v>37050</v>
-      </c>
-      <c r="J19" s="84">
+        <v>34050</v>
+      </c>
+      <c r="K19" s="77">
         <f>'dette unite'!$D$4</f>
-        <v>37050</v>
-      </c>
-      <c r="K19" s="84">
+        <v>34050</v>
+      </c>
+      <c r="L19" s="77">
         <f>'dette unite'!$D$4</f>
-        <v>37050</v>
-      </c>
-      <c r="L19" s="84">
-        <f>'dette unite'!$D$4</f>
-        <v>37050</v>
+        <v>34050</v>
       </c>
       <c r="M19" s="67">
         <f>'dette unite'!$D$4</f>
-        <v>37050</v>
+        <v>34050</v>
       </c>
       <c r="N19" s="67">
         <f>'dette unite'!$D$4</f>
-        <v>37050</v>
+        <v>34050</v>
       </c>
       <c r="O19" s="67">
         <f>'dette unite'!$D$4</f>
-        <v>37050</v>
+        <v>34050</v>
       </c>
       <c r="P19" s="67">
         <f>'dette unite'!$D$4</f>
-        <v>37050</v>
+        <v>34050</v>
       </c>
       <c r="Q19" s="67"/>
       <c r="R19" s="67"/>
@@ -18249,67 +18235,67 @@
     </row>
     <row r="20" spans="1:932" s="57" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="62" t="s">
-        <v>97</v>
-      </c>
-      <c r="B20" s="85">
+        <v>93</v>
+      </c>
+      <c r="B20" s="78">
         <f>B18+B19</f>
         <v>70000</v>
       </c>
-      <c r="C20" s="86">
+      <c r="C20" s="79">
         <f t="shared" ref="C20:P20" si="3">C18+C19</f>
         <v>44247</v>
       </c>
-      <c r="D20" s="86">
+      <c r="D20" s="79">
         <f t="shared" si="3"/>
         <v>110977.04000000001</v>
       </c>
-      <c r="E20" s="86">
+      <c r="E20" s="79">
         <f t="shared" si="3"/>
-        <v>37050</v>
-      </c>
-      <c r="F20" s="86">
+        <v>34050</v>
+      </c>
+      <c r="F20" s="79">
         <f t="shared" si="3"/>
-        <v>37050</v>
-      </c>
-      <c r="G20" s="86">
+        <v>34050</v>
+      </c>
+      <c r="G20" s="79">
         <f t="shared" si="3"/>
-        <v>37050</v>
-      </c>
-      <c r="H20" s="86">
+        <v>34050</v>
+      </c>
+      <c r="H20" s="79">
         <f t="shared" si="3"/>
-        <v>37050</v>
-      </c>
-      <c r="I20" s="86">
+        <v>34050</v>
+      </c>
+      <c r="I20" s="79">
         <f t="shared" si="3"/>
-        <v>37050</v>
-      </c>
-      <c r="J20" s="86">
+        <v>34050</v>
+      </c>
+      <c r="J20" s="79">
         <f t="shared" si="3"/>
-        <v>37050</v>
-      </c>
-      <c r="K20" s="86">
+        <v>34050</v>
+      </c>
+      <c r="K20" s="79">
         <f t="shared" si="3"/>
-        <v>37050</v>
-      </c>
-      <c r="L20" s="86">
+        <v>34050</v>
+      </c>
+      <c r="L20" s="79">
         <f t="shared" si="3"/>
-        <v>37050</v>
+        <v>34050</v>
       </c>
       <c r="M20" s="68">
         <f t="shared" si="3"/>
-        <v>37050</v>
+        <v>34050</v>
       </c>
       <c r="N20" s="68">
         <f t="shared" si="3"/>
-        <v>37050</v>
+        <v>34050</v>
       </c>
       <c r="O20" s="68">
         <f t="shared" si="3"/>
-        <v>37050</v>
+        <v>34050</v>
       </c>
       <c r="P20" s="68">
         <f t="shared" si="3"/>
-        <v>37050</v>
+        <v>34050</v>
       </c>
       <c r="Q20" s="68"/>
       <c r="R20" s="68"/>
@@ -24373,10 +24359,10 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:E853"/>
+  <dimension ref="A1:E851"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A9" sqref="A9:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24385,13 +24371,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="84" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="63" t="s">
@@ -24415,16 +24401,16 @@
         <v>83</v>
       </c>
       <c r="B4" s="64">
-        <f>SUM(B5:B2000)</f>
-        <v>130000</v>
+        <f>SUM(B5:B1998)</f>
+        <v>120000</v>
       </c>
       <c r="C4" s="64">
-        <f>SUM(C5:C2000)</f>
+        <f>SUM(C5:C1998)</f>
         <v>0</v>
       </c>
       <c r="D4" s="64">
         <f>B4-C4</f>
-        <v>130000</v>
+        <v>120000</v>
       </c>
       <c r="E4" s="64"/>
     </row>
@@ -24439,7 +24425,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="63">
-        <f t="shared" ref="D5:D28" si="0">B5-C5</f>
+        <f t="shared" ref="D5:D26" si="0">B5-C5</f>
         <v>15000</v>
       </c>
       <c r="E5" s="63"/>
@@ -24490,43 +24476,35 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="63" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="B9" s="63">
-        <v>5000</v>
+        <v>70000</v>
       </c>
       <c r="C9" s="63"/>
       <c r="D9" s="63">
         <f t="shared" si="0"/>
-        <v>5000</v>
+        <v>70000</v>
       </c>
       <c r="E9" s="63"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="B10" s="63">
-        <v>5000</v>
-      </c>
+      <c r="A10" s="63"/>
+      <c r="B10" s="63"/>
       <c r="C10" s="63"/>
       <c r="D10" s="63">
         <f t="shared" si="0"/>
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="E10" s="63"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="63" t="s">
-        <v>106</v>
-      </c>
-      <c r="B11" s="63">
-        <v>70000</v>
-      </c>
+      <c r="A11" s="63"/>
+      <c r="B11" s="63"/>
       <c r="C11" s="63"/>
       <c r="D11" s="63">
         <f t="shared" si="0"/>
-        <v>70000</v>
+        <v>0</v>
       </c>
       <c r="E11" s="63"/>
     </row>
@@ -24684,20 +24662,14 @@
       <c r="A27" s="63"/>
       <c r="B27" s="63"/>
       <c r="C27" s="63"/>
-      <c r="D27" s="63">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D27" s="63"/>
       <c r="E27" s="63"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="63"/>
       <c r="B28" s="63"/>
       <c r="C28" s="63"/>
-      <c r="D28" s="63">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D28" s="63"/>
       <c r="E28" s="63"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -30460,20 +30432,6 @@
       <c r="C851" s="63"/>
       <c r="D851" s="63"/>
       <c r="E851" s="63"/>
-    </row>
-    <row r="852" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A852" s="63"/>
-      <c r="B852" s="63"/>
-      <c r="C852" s="63"/>
-      <c r="D852" s="63"/>
-      <c r="E852" s="63"/>
-    </row>
-    <row r="853" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A853" s="63"/>
-      <c r="B853" s="63"/>
-      <c r="C853" s="63"/>
-      <c r="D853" s="63"/>
-      <c r="E853" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -30488,10 +30446,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:E1066"/>
+  <dimension ref="A1:E1064"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30500,13 +30458,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="84" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="63" t="s">
@@ -30530,16 +30488,16 @@
         <v>83</v>
       </c>
       <c r="B4" s="64">
-        <f>SUM(B5:B1998)</f>
-        <v>39550</v>
+        <f>SUM(B5:B1996)</f>
+        <v>37550</v>
       </c>
       <c r="C4" s="64">
-        <f>SUM(C5:C1998)</f>
-        <v>2500</v>
+        <f>SUM(C5:C1996)</f>
+        <v>3500</v>
       </c>
       <c r="D4" s="64">
         <f>B4-C4</f>
-        <v>37050</v>
+        <v>34050</v>
       </c>
       <c r="E4" s="64"/>
     </row>
@@ -30554,7 +30512,7 @@
         <v>2500</v>
       </c>
       <c r="D5" s="63">
-        <f t="shared" ref="D5:D25" si="0">B5-C5</f>
+        <f t="shared" ref="D5:D23" si="0">B5-C5</f>
         <v>3600</v>
       </c>
       <c r="E5" s="63"/>
@@ -30594,46 +30552,46 @@
         <v>88</v>
       </c>
       <c r="B8" s="63">
-        <v>1000</v>
+        <v>2200</v>
       </c>
       <c r="C8" s="63"/>
       <c r="D8" s="63">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>2200</v>
       </c>
       <c r="E8" s="63"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="63" t="s">
-        <v>89</v>
+        <v>33</v>
       </c>
       <c r="B9" s="63">
-        <v>1000</v>
+        <v>4000</v>
       </c>
       <c r="C9" s="63"/>
       <c r="D9" s="63">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>4000</v>
       </c>
       <c r="E9" s="63"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="63" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B10" s="63">
-        <v>2200</v>
+        <v>3000</v>
       </c>
       <c r="C10" s="63"/>
       <c r="D10" s="63">
         <f t="shared" si="0"/>
-        <v>2200</v>
+        <v>3000</v>
       </c>
       <c r="E10" s="63"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="63" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="B11" s="63">
         <v>4000</v>
@@ -30647,71 +30605,65 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="63" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="B12" s="63">
-        <v>3000</v>
+        <v>8250</v>
       </c>
       <c r="C12" s="63"/>
       <c r="D12" s="63">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>8250</v>
       </c>
       <c r="E12" s="63"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B13" s="63">
-        <v>4000</v>
-      </c>
-      <c r="C13" s="63"/>
+        <v>3500</v>
+      </c>
+      <c r="C13" s="63">
+        <v>1000</v>
+      </c>
       <c r="D13" s="63">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>2500</v>
       </c>
       <c r="E13" s="63"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="63" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="B14" s="63">
-        <v>8250</v>
+        <v>2000</v>
       </c>
       <c r="C14" s="63"/>
       <c r="D14" s="63">
         <f t="shared" si="0"/>
-        <v>8250</v>
+        <v>2000</v>
       </c>
       <c r="E14" s="63"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="63" t="s">
-        <v>95</v>
-      </c>
-      <c r="B15" s="63">
-        <v>3500</v>
-      </c>
+      <c r="A15" s="63"/>
+      <c r="B15" s="63"/>
       <c r="C15" s="63"/>
       <c r="D15" s="63">
         <f t="shared" si="0"/>
-        <v>3500</v>
+        <v>0</v>
       </c>
       <c r="E15" s="63"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="63" t="s">
-        <v>107</v>
-      </c>
-      <c r="B16" s="63">
-        <v>2000</v>
-      </c>
+      <c r="A16" s="63"/>
+      <c r="B16" s="63"/>
       <c r="C16" s="63"/>
       <c r="D16" s="63">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="E16" s="63"/>
     </row>
@@ -30789,20 +30741,14 @@
       <c r="A24" s="63"/>
       <c r="B24" s="63"/>
       <c r="C24" s="63"/>
-      <c r="D24" s="63">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D24" s="63"/>
       <c r="E24" s="63"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="63"/>
       <c r="B25" s="63"/>
       <c r="C25" s="63"/>
-      <c r="D25" s="63">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D25" s="63"/>
       <c r="E25" s="63"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -38077,20 +38023,6 @@
       <c r="C1064" s="63"/>
       <c r="D1064" s="63"/>
       <c r="E1064" s="63"/>
-    </row>
-    <row r="1065" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1065" s="63"/>
-      <c r="B1065" s="63"/>
-      <c r="C1065" s="63"/>
-      <c r="D1065" s="63"/>
-      <c r="E1065" s="63"/>
-    </row>
-    <row r="1066" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1066" s="63"/>
-      <c r="B1066" s="63"/>
-      <c r="C1066" s="63"/>
-      <c r="D1066" s="63"/>
-      <c r="E1066" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -38104,8 +38036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:JJ58"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AD1" activePane="topRight" state="frozen"/>
+    <sheetView topLeftCell="A24" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AE12" sqref="AE12"/>
     </sheetView>
   </sheetViews>
@@ -44086,7 +44018,7 @@
         <v>24</v>
       </c>
       <c r="V26" s="30" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="W26" s="30" t="s">
         <v>24</v>
@@ -44402,7 +44334,7 @@
       </c>
       <c r="U27" s="39"/>
       <c r="V27" s="30" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="W27" s="30"/>
       <c r="X27" s="30"/>
@@ -52563,14 +52495,14 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="76"/>
-      <c r="B19" s="77"/>
-      <c r="C19" s="78"/>
+      <c r="A19" s="85"/>
+      <c r="B19" s="86"/>
+      <c r="C19" s="87"/>
     </row>
     <row r="20" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="79"/>
-      <c r="B20" s="80"/>
-      <c r="C20" s="81"/>
+      <c r="A20" s="88"/>
+      <c r="B20" s="89"/>
+      <c r="C20" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>